<commit_message>
Added the program upload system, fixed some login issues, edited the constants, fixed some api's functions
</commit_message>
<xml_diff>
--- a/app/scripts/Exams_Table.xlsx
+++ b/app/scripts/Exams_Table.xlsx
@@ -52,100 +52,100 @@
     <t>9AM - 12PM</t>
   </si>
   <si>
+    <t>GEN33</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
+    <t>ECC20</t>
+  </si>
+  <si>
+    <t>ECC52</t>
+  </si>
+  <si>
+    <t>GEN44</t>
+  </si>
+  <si>
+    <t>ECC39</t>
+  </si>
+  <si>
+    <t>HUM305</t>
+  </si>
+  <si>
+    <t>MECH16</t>
+  </si>
+  <si>
+    <t>ECC18</t>
+  </si>
+  <si>
+    <t>ECC47</t>
+  </si>
+  <si>
+    <t>ECC07</t>
+  </si>
+  <si>
+    <t>ECC49</t>
+  </si>
+  <si>
+    <t>GEN11</t>
+  </si>
+  <si>
+    <t>MECH14</t>
+  </si>
+  <si>
+    <t>ECC50</t>
+  </si>
+  <si>
+    <t>GEN41</t>
+  </si>
+  <si>
+    <t>ECC40</t>
+  </si>
+  <si>
+    <t>ECC37</t>
+  </si>
+  <si>
+    <t>ECC23</t>
+  </si>
+  <si>
+    <t>MECH24</t>
+  </si>
+  <si>
+    <t>ECC45</t>
+  </si>
+  <si>
+    <t>ECC413</t>
+  </si>
+  <si>
+    <t>ECC31</t>
+  </si>
+  <si>
+    <t>ECC35</t>
+  </si>
+  <si>
+    <t>ECC25</t>
+  </si>
+  <si>
+    <t>ECC48</t>
+  </si>
+  <si>
+    <t>ECC53</t>
+  </si>
+  <si>
+    <t>GEN05</t>
+  </si>
+  <si>
+    <t>GEN26</t>
+  </si>
+  <si>
+    <t>ECC34</t>
+  </si>
+  <si>
     <t>ECC32</t>
   </si>
   <si>
-    <t>MECH14</t>
-  </si>
-  <si>
-    <t>ECC50</t>
-  </si>
-  <si>
-    <t>ECC18</t>
-  </si>
-  <si>
-    <t>GEN11</t>
-  </si>
-  <si>
-    <t>ECC413</t>
-  </si>
-  <si>
-    <t>GEN41</t>
-  </si>
-  <si>
-    <t>ECC53</t>
-  </si>
-  <si>
-    <t>ECC31</t>
-  </si>
-  <si>
     <t>GEN04</t>
-  </si>
-  <si>
-    <t>ECC23</t>
-  </si>
-  <si>
-    <t>ECC37</t>
-  </si>
-  <si>
-    <t>ECC07</t>
-  </si>
-  <si>
-    <t>ECC45</t>
-  </si>
-  <si>
-    <t>ECC47</t>
-  </si>
-  <si>
-    <t>GEN44</t>
-  </si>
-  <si>
-    <t>GEN26</t>
-  </si>
-  <si>
-    <t>ECC40</t>
-  </si>
-  <si>
-    <t>ECC49</t>
-  </si>
-  <si>
-    <t>ECC25</t>
-  </si>
-  <si>
-    <t>ECC48</t>
-  </si>
-  <si>
-    <t>GEN33</t>
-  </si>
-  <si>
-    <t>ECC52</t>
-  </si>
-  <si>
-    <t>ECC20</t>
-  </si>
-  <si>
-    <t>MECH16</t>
-  </si>
-  <si>
-    <t>HUM305</t>
-  </si>
-  <si>
-    <t>ECC39</t>
-  </si>
-  <si>
-    <t>ECC34</t>
-  </si>
-  <si>
-    <t>MECH24</t>
-  </si>
-  <si>
-    <t>ECC35</t>
-  </si>
-  <si>
-    <t>GEN05</t>
   </si>
 </sst>
 </file>
@@ -526,31 +526,31 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -558,34 +558,34 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -593,34 +593,34 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -628,34 +628,34 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -663,34 +663,34 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -698,34 +698,34 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -733,34 +733,34 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
       <c r="K8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -768,34 +768,34 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -803,34 +803,34 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -838,34 +838,34 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="K11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -873,34 +873,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -908,34 +908,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -943,34 +943,34 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -978,34 +978,34 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a page for time tables , finished the lecture time table generation page , modified the finished courses api to return each semster courses
</commit_message>
<xml_diff>
--- a/app/scripts/Exams_Table.xlsx
+++ b/app/scripts/Exams_Table.xlsx
@@ -1,77 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Graduation-Project\Website\intelligent-college-timetable-scheduler(test)\app\scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4C1BD6-25AF-451C-8D61-C413C50F506F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="1320" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Day-Time</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test7</t>
-  </si>
-  <si>
-    <t>test8</t>
-  </si>
-  <si>
-    <t>test9</t>
-  </si>
-  <si>
-    <t>test10</t>
+    <t>Hall 1</t>
+  </si>
+  <si>
+    <t>Hall 2</t>
+  </si>
+  <si>
+    <t>Hall 5</t>
   </si>
   <si>
     <t>9AM - 12PM</t>
   </si>
   <si>
+    <t>CD222</t>
+  </si>
+  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>CIE4819</t>
-  </si>
-  <si>
-    <t>CIE4816</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,14 +78,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,27 +156,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,24 +190,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,19 +365,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,61 +385,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some bugs, enhanced the UI, filled the database with test data
</commit_message>
<xml_diff>
--- a/app/scripts/Exams_Table.xlsx
+++ b/app/scripts/Exams_Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Day-Time</t>
   </si>
@@ -31,10 +31,58 @@
     <t>9AM - 12PM</t>
   </si>
   <si>
-    <t>CD222</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>MEC0811</t>
+  </si>
+  <si>
+    <t>CIE2802</t>
+  </si>
+  <si>
+    <t>GEN0801</t>
+  </si>
+  <si>
+    <t>GEN0810</t>
+  </si>
+  <si>
+    <t>GEN0807</t>
+  </si>
+  <si>
+    <t>CIE3801</t>
+  </si>
+  <si>
+    <t>GEN1801</t>
+  </si>
+  <si>
+    <t>GEN0806</t>
+  </si>
+  <si>
+    <t>CIE3804</t>
+  </si>
+  <si>
+    <t>CIE1803</t>
+  </si>
+  <si>
+    <t>GEN1805</t>
+  </si>
+  <si>
+    <t>CIE4818</t>
+  </si>
+  <si>
+    <t>GEN2810</t>
+  </si>
+  <si>
+    <t>GEN1809</t>
+  </si>
+  <si>
+    <t>GEN0809</t>
+  </si>
+  <si>
+    <t>GEN0802</t>
+  </si>
+  <si>
+    <t>CIE1808</t>
+  </si>
+  <si>
+    <t>POW1804</t>
   </si>
 </sst>
 </file>
@@ -366,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,7 +445,77 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing some bugs and added a page for current students courses
</commit_message>
<xml_diff>
--- a/app/scripts/Exams_Table.xlsx
+++ b/app/scripts/Exams_Table.xlsx
@@ -31,58 +31,58 @@
     <t>9AM - 12PM</t>
   </si>
   <si>
+    <t>GEN0802</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>GEN0810</t>
+  </si>
+  <si>
+    <t>CIE4818</t>
+  </si>
+  <si>
+    <t>POW1804</t>
+  </si>
+  <si>
+    <t>GEN1805</t>
+  </si>
+  <si>
+    <t>GEN0806</t>
+  </si>
+  <si>
+    <t>CIE1808</t>
+  </si>
+  <si>
+    <t>GEN1809</t>
+  </si>
+  <si>
+    <t>CIE1803</t>
+  </si>
+  <si>
+    <t>GEN0807</t>
+  </si>
+  <si>
+    <t>GEN1801</t>
+  </si>
+  <si>
+    <t>GEN2810</t>
+  </si>
+  <si>
+    <t>CIE3804</t>
+  </si>
+  <si>
+    <t>GEN0809</t>
+  </si>
+  <si>
+    <t>CIE2802</t>
+  </si>
+  <si>
     <t>MEC0811</t>
   </si>
   <si>
-    <t>CIE2802</t>
-  </si>
-  <si>
     <t>GEN0801</t>
-  </si>
-  <si>
-    <t>GEN0810</t>
-  </si>
-  <si>
-    <t>GEN0807</t>
-  </si>
-  <si>
-    <t>CIE3801</t>
-  </si>
-  <si>
-    <t>GEN1801</t>
-  </si>
-  <si>
-    <t>GEN0806</t>
-  </si>
-  <si>
-    <t>CIE3804</t>
-  </si>
-  <si>
-    <t>CIE1803</t>
-  </si>
-  <si>
-    <t>GEN1805</t>
-  </si>
-  <si>
-    <t>CIE4818</t>
-  </si>
-  <si>
-    <t>GEN2810</t>
-  </si>
-  <si>
-    <t>GEN1809</t>
-  </si>
-  <si>
-    <t>GEN0809</t>
-  </si>
-  <si>
-    <t>GEN0802</t>
-  </si>
-  <si>
-    <t>CIE1808</t>
-  </si>
-  <si>
-    <t>POW1804</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Enhanced the timetable generation process
</commit_message>
<xml_diff>
--- a/app/scripts/Exams_Table.xlsx
+++ b/app/scripts/Exams_Table.xlsx
@@ -31,55 +31,55 @@
     <t>9AM - 12PM</t>
   </si>
   <si>
+    <t>GEN2810</t>
+  </si>
+  <si>
+    <t>CIE2802</t>
+  </si>
+  <si>
+    <t>CIE4818</t>
+  </si>
+  <si>
+    <t>POW1804</t>
+  </si>
+  <si>
+    <t>GEN0809</t>
+  </si>
+  <si>
+    <t>GEN1805</t>
+  </si>
+  <si>
+    <t>GEN0807</t>
+  </si>
+  <si>
+    <t>CIE1808</t>
+  </si>
+  <si>
+    <t>MEC0811</t>
+  </si>
+  <si>
+    <t>CIE1803</t>
+  </si>
+  <si>
+    <t>GEN1809</t>
+  </si>
+  <si>
     <t>GEN0802</t>
   </si>
   <si>
+    <t>GEN1801</t>
+  </si>
+  <si>
+    <t>CIE3804</t>
+  </si>
+  <si>
+    <t>GEN0806</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
     <t>GEN0810</t>
-  </si>
-  <si>
-    <t>CIE4818</t>
-  </si>
-  <si>
-    <t>POW1804</t>
-  </si>
-  <si>
-    <t>GEN1805</t>
-  </si>
-  <si>
-    <t>GEN0806</t>
-  </si>
-  <si>
-    <t>CIE1808</t>
-  </si>
-  <si>
-    <t>GEN1809</t>
-  </si>
-  <si>
-    <t>CIE1803</t>
-  </si>
-  <si>
-    <t>GEN0807</t>
-  </si>
-  <si>
-    <t>GEN1801</t>
-  </si>
-  <si>
-    <t>GEN2810</t>
-  </si>
-  <si>
-    <t>CIE3804</t>
-  </si>
-  <si>
-    <t>GEN0809</t>
-  </si>
-  <si>
-    <t>CIE2802</t>
-  </si>
-  <si>
-    <t>MEC0811</t>
   </si>
   <si>
     <t>GEN0801</t>

</xml_diff>